<commit_message>
General updates, added validation script, added examples
</commit_message>
<xml_diff>
--- a/ComboList&Data.xlsx
+++ b/ComboList&Data.xlsx
@@ -450,11 +450,11 @@
   </sheetPr>
   <dimension ref="A1:I123"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A105" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9:G123"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.67"/>
@@ -560,7 +560,7 @@
       <c r="F5" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -583,7 +583,7 @@
       <c r="F6" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="G6" s="1" t="n">
+      <c r="G6" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -629,7 +629,7 @@
       <c r="F8" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="G8" s="1" t="n">
+      <c r="G8" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -652,7 +652,7 @@
       <c r="F9" s="1" t="n">
         <v>142</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -721,7 +721,7 @@
       <c r="F12" s="0" t="n">
         <v>142</v>
       </c>
-      <c r="G12" s="1" t="n">
+      <c r="G12" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -790,7 +790,7 @@
       <c r="F15" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="G15" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I15" s="1"/>
@@ -814,7 +814,7 @@
       <c r="F16" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="G16" s="1" t="n">
+      <c r="G16" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -860,7 +860,7 @@
       <c r="F18" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="G18" s="1" t="n">
+      <c r="G18" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -883,7 +883,7 @@
       <c r="F19" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="G19" s="0" t="n">
+      <c r="G19" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -952,7 +952,7 @@
       <c r="F22" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="G22" s="1" t="n">
+      <c r="G22" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1021,7 +1021,7 @@
       <c r="F25" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="G25" s="0" t="n">
+      <c r="G25" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1044,7 +1044,7 @@
       <c r="F26" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="G26" s="1" t="n">
+      <c r="G26" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1090,7 +1090,7 @@
       <c r="F28" s="0" t="n">
         <v>38</v>
       </c>
-      <c r="G28" s="1" t="n">
+      <c r="G28" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1113,7 +1113,7 @@
       <c r="F29" s="0" t="n">
         <v>38</v>
       </c>
-      <c r="G29" s="0" t="n">
+      <c r="G29" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1182,7 +1182,7 @@
       <c r="F32" s="0" t="n">
         <v>38</v>
       </c>
-      <c r="G32" s="1" t="n">
+      <c r="G32" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1251,7 +1251,7 @@
       <c r="F35" s="0" t="n">
         <v>57</v>
       </c>
-      <c r="G35" s="0" t="n">
+      <c r="G35" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1274,7 +1274,7 @@
       <c r="F36" s="0" t="n">
         <v>57</v>
       </c>
-      <c r="G36" s="1" t="n">
+      <c r="G36" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1320,7 +1320,7 @@
       <c r="F38" s="0" t="n">
         <v>57</v>
       </c>
-      <c r="G38" s="1" t="n">
+      <c r="G38" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       <c r="F39" s="0" t="n">
         <v>57</v>
       </c>
-      <c r="G39" s="0" t="n">
+      <c r="G39" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1412,7 +1412,7 @@
       <c r="F42" s="0" t="n">
         <v>85</v>
       </c>
-      <c r="G42" s="1" t="n">
+      <c r="G42" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1481,7 +1481,7 @@
       <c r="F45" s="0" t="n">
         <v>85</v>
       </c>
-      <c r="G45" s="0" t="n">
+      <c r="G45" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1504,7 +1504,7 @@
       <c r="F46" s="0" t="n">
         <v>85</v>
       </c>
-      <c r="G46" s="1" t="n">
+      <c r="G46" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1550,7 +1550,7 @@
       <c r="F48" s="0" t="n">
         <v>85</v>
       </c>
-      <c r="G48" s="1" t="n">
+      <c r="G48" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1573,7 +1573,7 @@
       <c r="F49" s="0" t="n">
         <v>85</v>
       </c>
-      <c r="G49" s="0" t="n">
+      <c r="G49" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1642,7 +1642,7 @@
       <c r="F52" s="1" t="n">
         <v>110</v>
       </c>
-      <c r="G52" s="1" t="n">
+      <c r="G52" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1711,7 +1711,7 @@
       <c r="F55" s="0" t="n">
         <v>110</v>
       </c>
-      <c r="G55" s="0" t="n">
+      <c r="G55" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1734,7 +1734,7 @@
       <c r="F56" s="0" t="n">
         <v>110</v>
       </c>
-      <c r="G56" s="1" t="n">
+      <c r="G56" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1780,7 +1780,7 @@
       <c r="F58" s="0" t="n">
         <v>110</v>
       </c>
-      <c r="G58" s="1" t="n">
+      <c r="G58" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1803,7 +1803,7 @@
       <c r="F59" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="G59" s="0" t="n">
+      <c r="G59" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1872,7 +1872,7 @@
       <c r="F62" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="G62" s="1" t="n">
+      <c r="G62" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1941,7 +1941,7 @@
       <c r="F65" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="G65" s="0" t="n">
+      <c r="G65" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1964,7 +1964,7 @@
       <c r="F66" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="G66" s="1" t="n">
+      <c r="G66" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2010,7 +2010,7 @@
       <c r="F68" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="G68" s="1" t="n">
+      <c r="G68" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2033,7 +2033,7 @@
       <c r="F69" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="G69" s="0" t="n">
+      <c r="G69" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2102,7 +2102,7 @@
       <c r="F72" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="G72" s="1" t="n">
+      <c r="G72" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2171,7 +2171,7 @@
       <c r="F75" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="G75" s="0" t="n">
+      <c r="G75" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2194,7 +2194,7 @@
       <c r="F76" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="G76" s="1" t="n">
+      <c r="G76" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2240,7 +2240,7 @@
       <c r="F78" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="G78" s="1" t="n">
+      <c r="G78" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2263,7 +2263,7 @@
       <c r="F79" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="G79" s="0" t="n">
+      <c r="G79" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2332,7 +2332,7 @@
       <c r="F82" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="G82" s="1" t="n">
+      <c r="G82" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2401,7 +2401,7 @@
       <c r="F85" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="G85" s="0" t="n">
+      <c r="G85" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2424,7 +2424,7 @@
       <c r="F86" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="G86" s="1" t="n">
+      <c r="G86" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2470,7 +2470,7 @@
       <c r="F88" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="G88" s="1" t="n">
+      <c r="G88" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2493,7 +2493,7 @@
       <c r="F89" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="G89" s="0" t="n">
+      <c r="G89" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2562,7 +2562,7 @@
       <c r="F92" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="G92" s="1" t="n">
+      <c r="G92" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2631,7 +2631,7 @@
       <c r="F95" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="G95" s="0" t="n">
+      <c r="G95" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       <c r="F96" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="G96" s="1" t="n">
+      <c r="G96" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2700,7 +2700,7 @@
       <c r="F98" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="G98" s="1" t="n">
+      <c r="G98" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2723,7 +2723,7 @@
       <c r="F99" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="G99" s="0" t="n">
+      <c r="G99" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2792,7 +2792,7 @@
       <c r="F102" s="0" t="n">
         <v>171</v>
       </c>
-      <c r="G102" s="1" t="n">
+      <c r="G102" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2861,7 +2861,7 @@
       <c r="F105" s="0" t="n">
         <v>65</v>
       </c>
-      <c r="G105" s="0" t="n">
+      <c r="G105" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2884,7 +2884,7 @@
       <c r="F106" s="0" t="n">
         <v>65</v>
       </c>
-      <c r="G106" s="1" t="n">
+      <c r="G106" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2930,7 +2930,7 @@
       <c r="F108" s="0" t="n">
         <v>65</v>
       </c>
-      <c r="G108" s="1" t="n">
+      <c r="G108" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2953,7 +2953,7 @@
       <c r="F109" s="0" t="n">
         <v>65</v>
       </c>
-      <c r="G109" s="0" t="n">
+      <c r="G109" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3022,7 +3022,7 @@
       <c r="F112" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="G112" s="1" t="n">
+      <c r="G112" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3091,7 +3091,7 @@
       <c r="F115" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="G115" s="0" t="n">
+      <c r="G115" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3114,7 +3114,7 @@
       <c r="F116" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="G116" s="1" t="n">
+      <c r="G116" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3160,7 +3160,7 @@
       <c r="F118" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="G118" s="1" t="n">
+      <c r="G118" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3184,7 +3184,7 @@
       <c r="F119" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="G119" s="0" t="n">
+      <c r="G119" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3232,7 +3232,7 @@
       <c r="F121" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="G121" s="0" t="n">
+      <c r="G121" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3280,7 +3280,7 @@
       <c r="F123" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="G123" s="0" t="n">
+      <c r="G123" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3303,10 +3303,10 @@
   <dimension ref="A1:G1107"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1073" activeCellId="0" sqref="C1073"/>
+      <selection pane="topLeft" activeCell="C1073" activeCellId="1" sqref="G9:G123 C1073"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.54"/>
@@ -20432,10 +20432,10 @@
   <dimension ref="A1:G533"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E91" activeCellId="0" sqref="E91"/>
+      <selection pane="topLeft" activeCell="E91" activeCellId="1" sqref="G9:G123 E91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.54"/>
@@ -28246,10 +28246,10 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G36" activeCellId="0" sqref="G36"/>
+      <selection pane="topLeft" activeCell="G36" activeCellId="0" sqref="G9:G123"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.28"/>

</xml_diff>